<commit_message>
Expanded groupby functionality to to include multi-field keys and developed associated tests.
</commit_message>
<xml_diff>
--- a/concero/tests/data/test_groupby_and_aggregate.xlsx
+++ b/concero/tests/data/test_groupby_and_aggregate.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="groupby" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="groupby_2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="4">
   <si>
     <t xml:space="preserve">a</t>
   </si>
@@ -46,6 +47,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -129,13 +131,13 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -207,4 +209,162 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="0" t="n">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>